<commit_message>
updated Registration center for spanish language.
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/registration_center.xlsx
+++ b/mosip_master/xlsx/registration_center.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A53625-DE9D-439F-B129-A687C25FA92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CA5E7-C346-4A90-9CEB-D704FCEE522A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:W96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U85" sqref="U85"/>
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8213,7 +8213,7 @@
         <v>45.245600000000003</v>
       </c>
       <c r="J96">
-        <v>14080</v>
+        <v>10114</v>
       </c>
       <c r="K96">
         <v>9663089998</v>

</xml_diff>